<commit_message>
updated matrix with terms
</commit_message>
<xml_diff>
--- a/Data/dmdu_classification_matrix_with_keywords.xlsx
+++ b/Data/dmdu_classification_matrix_with_keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strep\Desktop\DMDU REG\Framework dmdi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/538fd21f0dfa6547/Escritorio/Caro/DMDU REG/Framework dmdi/Scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD7B046-6D6A-4CC2-942A-DE7CD2054924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{8FD7B046-6D6A-4CC2-942A-DE7CD2054924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A32342CA-C9E0-4A9F-9E3E-DB2CAC040D90}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uncertainty_Types" sheetId="1" r:id="rId1"/>
@@ -259,24 +259,12 @@
     <t>unknown unknowns, radical uncertainty, no information, irreducible, black swan, highly unpredictable, inconceivable, no information, no probabilities, radical uncertainty, unforeseeable, unknown unknowns, unquantifiable</t>
   </si>
   <si>
-    <t>assumptions about reality, hidden structures, ontology, model structure, assumptions about reality, causal ambiguity, emergent properties, existential uncertainty, hidden structures, model blindness, what exists is unclear</t>
-  </si>
-  <si>
-    <t>intentional ignorance, lack of transparency, political interference, agency omission, agenda-driven uncertainty, intentional ignorance, lack of transparency, political distortion, selective disclosure, strategic ignorance, withheld data</t>
-  </si>
-  <si>
     <t>deep uncertainty, structural disagreement, model conflict, unknown probabilities, conflicting evidence, deep uncertainty, disagreement on assumptions, model divergence, multiple plausible futures, scenario divergence, structural disagreement, unknown</t>
   </si>
   <si>
-    <t>lack of knowledge, imperfect knowledge, data scarcity, limited information, data scarcity, imperfect knowledge, incomplete evidence, information gaps, lack of knowledge, limited understanding, poor data quality, uncertain facts, uncertainty due to</t>
-  </si>
-  <si>
     <t>semantic ambiguity, vague expressions, unclear meaning, linguistic fuzziness, ambiguous wording, language uncertainty, misleading terminology, semantic ambiguity, unclear terms, vague expressions</t>
   </si>
   <si>
-    <t>normative uncertainty, value disagreement, ethical dilemmas, future values, conflicting preferences, divergent goals, ethical conflict, moral ambiguity, norm clashes, value disagreement</t>
-  </si>
-  <si>
     <t>multiple frames, conflicting visions, desirable futures, ambiguity, alternative meanings, conflicting visions, desirable futures, interpretive uncertainty, multiple frames, unclear framing</t>
   </si>
   <si>
@@ -286,33 +274,12 @@
     <t>infrastructure, energy system, urban planner, carbon sources, contaminant release, emission actors, emitters, environmental burden, industrial discharge, polluters, waste producers</t>
   </si>
   <si>
-    <t>citizen, user, public, consumer, communities served, ecosystem beneficiaries, indirect users, public users, resource consumers, resource dependents, service recipients, users</t>
-  </si>
-  <si>
-    <t>community, vulnerable, ngo, affected, displaced people, downstream users, exposed populations, impacted communities, negatively affected, socially affected groups, those bearing costs, vulnerable populations</t>
-  </si>
-  <si>
-    <t>government, policy maker, regulator, agency,   authorities, bureaucracies, compliance bodies, environmental agencies, government, lawmakers, municipalities, policy makers</t>
-  </si>
-  <si>
-    <t>media, academic, influencer, expert, advocacy organizations, civil society groups, consultants, lobbyists, media, opinion leaders, researchers, technical experts, think tanks</t>
-  </si>
-  <si>
     <t>inform, bulletin, communication, awareness, access to information, communication, data provision, information sharing, informing stakeholders, knowledge dissemination, public announcements, public notice, transparent</t>
   </si>
   <si>
-    <t>consultation, survey, hearing, public opinion, comment periods, deliberative polling, participatory feedback, public hearings, public input, questionnaires, stakeholder feedback, surveys</t>
-  </si>
-  <si>
     <t>collaboration, participatory, workshop, mapping, co-design, co-production, joint planning, multi-stakeholder dialogue, partnerships, shared responsibility, stakeholder involvement in implementation, working groups</t>
   </si>
   <si>
-    <t>joint decision, deliberation, multicriteria, jury, consensus-building, deliberative decision-making, joint decision-making, negotiated agreements, participatory governance, shared decision-making</t>
-  </si>
-  <si>
-    <t>empowerment, delegation, co-management, local authority, autonomous decision-making, citizen control, community-led, delegated authority, grassroots decision-making, power transfer, self-determination, stakeholder control</t>
-  </si>
-  <si>
     <t>data gap, no monitoring, missing records,  controversy, uncertainty of knowledge</t>
   </si>
   <si>
@@ -322,37 +289,70 @@
     <t>local knowledge, community input, traditional knowledge,  controversy, uncertainty of knowledge</t>
   </si>
   <si>
-    <t>rigid law, outdated policy, inflexible regulation, administrative obstacles, bureaucratic inertia, institutional fragmentation, institutional resistance, lack of coordination, lack of enforcement, poor governance, regulatory misalignment, rigid structures</t>
-  </si>
-  <si>
-    <t>political shift, discontinuity, administration change, administrative obstacles, bureaucratic inertia, institutional fragmentation, institutional resistance, lack of coordination, lack of enforcement, poor governance, regulatory misalignment, rigid structures</t>
-  </si>
-  <si>
-    <t>overlap, role confusion, jurisdiction conflict, administrative obstacles, bureaucratic inertia, institutional fragmentation, institutional resistance, lack of coordination, lack of enforcement, poor governance, regulatory misalignment, rigid structures</t>
-  </si>
-  <si>
-    <t>access inequality, participation barrier, representation gap, community disengagement, conflicting interests, cultural barriers, lack of trust, low participation, public resistance, social fragmentation, social inequality, stakeholder conflict</t>
-  </si>
-  <si>
-    <t>scaling difficulty, large-scale participation, community disengagement, conflicting interests, cultural barriers, lack of trust, low participation, public resistance, social fragmentation, social inequality, stakeholder conflict</t>
-  </si>
-  <si>
-    <t>low trust, illegitimacy, social distrust, community disengagement, conflicting interests, cultural barriers, lack of trust, low participation, public resistance, social fragmentation, social inequality, stakeholder conflict</t>
-  </si>
-  <si>
-    <t>complex model, over-reliance on quant, inapplicable simulation, inadequate frameworks, lack of data, method mismatch, model uncertainty, modeling assumptions, parameter sensitivity, poor calibration, technical complexity, tool limitations</t>
-  </si>
-  <si>
-    <t>no local tool, context-specific approach, KSIM, inadequate frameworks, lack of data, method mismatch, model uncertainty, modeling assumptions, parameter sensitivity, poor calibration, technical complexity, tool limitations</t>
-  </si>
-  <si>
-    <t>translation gap, policy uptake barrier, inadequate frameworks, lack of data, method mismatch, model uncertainty, modeling assumptions, parameter sensitivity, poor calibration, technical complexity, tool limitations</t>
-  </si>
-  <si>
-    <t>short-term focus, electoral pressure, changing baselines, delayed impacts, future unpredictability, intergenerational issues, lag effects, long time horizons, policy cycles, short-termism, temporal mismatch</t>
-  </si>
-  <si>
-    <t>path dependency, institutional inertia, changing baselines, delayed impacts, future unpredictability, intergenerational issues, lag effects, long time horizons, policy cycles, short-termism, temporal mismatch</t>
+    <t>rigid law, outdated policy, inflexible regulation, administrative obstacles, bureaucratic inertia, institutional fragmentation, institutional resistance, lack of coordination, lack of enforcement, poor governance, regulatory, policy turnover, electoral cycle misalignment, rigid structures, alternancia política, alternância política, institutional fragility, policy instability</t>
+  </si>
+  <si>
+    <t>political shift, discontinuity, administration change, administrative obstacles, bureaucratic inertia, institutional fragmentation, institutional resistance, lack of coordination, lack of enforcement, poor governance, regulatory, policy turnover, electoral cycle misalignment, rigid structures, alternancia política, alternância política, institutional fragility, policy instability misalignment, rigid structures</t>
+  </si>
+  <si>
+    <t>overlap, role confusion, jurisdiction conflict, administrative obstacles, bureaucratic inertia, institutional fragmentation, institutional resistance, lack of coordination, lack of enforcement, poor governance, regulatory, policy turnover, electoral cycle misalignment, rigid structures, alternancia política, alternância política, institutional fragility, policy instability misalignment, rigid structures</t>
+  </si>
+  <si>
+    <t>complex model, over-reliance on quant, inapplicable simulation, inadequate frameworks, lack of data, method mismatch, model uncertainty, modeling assumptions, parameter sensitivity, poor calibration, technical, methodological challenges, complejidad del modelo, complexidade do modelo, technical uncertainty, data limitations complexity, tool limitations</t>
+  </si>
+  <si>
+    <t>no local tool, context-specific approach, KSIM, inadequate frameworks, lack of data, method mismatch, model uncertainty, modeling assumptions, parameter sensitivity, poor calibration, technical complexity, tool limitations, methodological challenges, complejidad del modelo, complexidade do modelo, technical uncertainty, data limitations</t>
+  </si>
+  <si>
+    <t>translation gap, policy uptake barrier, inadequate frameworks, lack of data, method mismatch, model uncertainty, modeling assumptions, parameter sensitivity, poor calibration, technical complexity, tool limitations, methodological challenges, complejidad del modelo, complexidade do modelo, technical uncertainty, data limitations</t>
+  </si>
+  <si>
+    <t>access inequality, participation barrier, representation gap, community disengagement, conflicting interests, cultural barriers, lack of trust, low participation, public resistance, social fragmentation, social inequality, legitimacy issues, social resistance, falta de confianza, falta de confiança, social acceptance, public perception stakeholder conflict</t>
+  </si>
+  <si>
+    <t>scaling difficulty, large-scale participation, community disengagement, conflicting interests, cultural barriers, lack of trust, low participation, public resistance, social fragmentation, social inequality, stakeholder conflict, legitimacy issues, social resistance, falta de confianza, falta de confiança, social acceptance, public perception</t>
+  </si>
+  <si>
+    <t>low trust, illegitimacy, social distrust, community disengagement, conflicting interests, cultural barriers, lack of trust, low participation, public resistance, social fragmentation, social inequality, stakeholder conflict, legitimacy issues, social resistance, falta de confianza, falta de confiança, social acceptance, public perception</t>
+  </si>
+  <si>
+    <t>short-term focus, electoral pressure, changing baselines, delayed impacts, future unpredictability, intergenerational issues, lag effects, long time horizons, policy cycles, short-termism, temporal mismatch, transaction costs, limited resources, altos costos, recursos limitados, altos custos, recursos limitados, cost-benefit trade-off, financial uncertainty</t>
+  </si>
+  <si>
+    <t>path dependency, institutional inertia, changing baselines, delayed impacts, future unpredictability, intergenerational issues, lag effects, long time horizons, policy cycles, short-termism, temporal mismatch, transaction costs, limited resources, altos costos, recursos limitados, altos custos, recursos limitados, cost-benefit trade-off, financial uncertainty</t>
+  </si>
+  <si>
+    <t>consultation, survey, hearing, public opinion, comment periods, deliberative polling, participatory feedback, public hearings, public input, questionnaires, stakeholder feedback, surveys, advisory process, information sharing, consulta, asesoría, consulta, assessoria, public consultation, consultation fórum</t>
+  </si>
+  <si>
+    <t>joint decision, deliberation, multicriteria, jury, consensus-building, deliberative decision-making, joint decision-making, negotiated agreements, participatory governance, shared decision-making, co-creation, shared governance, cogestión, toma conjunta, cogestão, decisão conjunta, deliberative democracy, co-production of knowledge</t>
+  </si>
+  <si>
+    <t>empowerment, delegation, co-management, local authority, autonomous decision-making, citizen control, community-led, delegated authority, grassroots decision-making, power transfer, self-determination, stakeholder, self-governance, autonomy, control ciudadano, autogestión, controle cidadão, autogestão, community empowerment, grassroots decision-making control</t>
+  </si>
+  <si>
+    <t>community, vulnerable, ngo, affected, displaced people, downstream users, exposed populations, impacted communities, negatively affected, socially affected groups, those bearing costs, vulnerable populations, local actors, grassroots organizations, actores locales, organizaciones de base, atores locais, organizações de base, multi-stakeholder process, participatory governan</t>
+  </si>
+  <si>
+    <t>citizen, user, public, consumer, communities served, ecosystem beneficiaries, indirect users, public users, resource consumers, resource dependents, service recipients, users, local actors, grassroots organizations, actores locales, organizaciones de base, atores locais, organizações de base, multi-stakeholder process, participatory governan</t>
+  </si>
+  <si>
+    <t>media, academic, influencer, expert, advocacy organizations, civil society groups, consultants, lobbyists, media, opinion leaders, researchers, technical experts, think tanks, industry, business actors, empresas, sector privado, empresas, setor privado, corporate governance, market actors</t>
+  </si>
+  <si>
+    <t>government, policy maker, regulator, agency,   authorities, bureaucracies, compliance bodies, environmental agencies, government, lawmakers, municipalities, policy makers, public authority, ministry, gobierno, autoridad, industry, business actors, empresas, sector privado, empresas, setor privado, corporate governance, market actors reguladora, governo, autoridade reguladora, policy entrepreneurs, regulatory agency</t>
+  </si>
+  <si>
+    <t>lack of knowledge, imperfect knowledge, data scarcity, limited information, data scarcity, imperfect knowledge, incomplete evidence, information gaps, lack of knowledge, limited understanding, poor data quality, uncertain, incomplete evidence, limited information, conocimiento imperfecto, falta de datos, conhecimento imperfeito, informação limitada, data scarcity, knowledge gaps facts, uncertainty due to</t>
+  </si>
+  <si>
+    <t>assumptions about reality, hidden structures, ontology, model structure, assumptions about reality, causal ambiguity, emergent properties, existential uncertainty, hidden structures, model blindness, what exists is unclear, deep structure, hidden dynamics, procesos desconocidos, processos desconhecidos, ontological uncertainty, system complexity</t>
+  </si>
+  <si>
+    <t>normative uncertainty, value disagreement, ethical dilemmas, future values, conflicting preferences, divergent goals, ethical conflict, moral ambiguity, norm clashes, value disagreement, value plurality, ethical debates, valores en conflicto, valores em conflito, normative ambiguity, social values</t>
+  </si>
+  <si>
+    <t>intentional ignorance, lack of transparency, political interference, agency omission, agenda-driven uncertainty, intentional ignorance, lack of transparency, political distortion, selective disclosure, strategic ignorance, governance challenges, asimetrías de poder, assimetrias de poder, political uncertainty, regime change withheld data</t>
   </si>
 </sst>
 </file>
@@ -718,19 +718,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="232.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="232.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -758,7 +758,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -769,10 +769,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -783,10 +783,10 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -797,10 +797,10 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -811,10 +811,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -825,10 +825,10 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -839,10 +839,10 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -853,7 +853,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -866,17 +866,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="193.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="193.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -887,7 +887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -895,10 +895,10 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -906,10 +906,10 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -917,10 +917,10 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -928,10 +928,10 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -939,10 +939,10 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -950,7 +950,7 @@
         <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -963,18 +963,18 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="208.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="208.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -988,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -999,10 +999,10 @@
         <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1013,10 +1013,10 @@
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1027,10 +1027,10 @@
         <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1041,10 +1041,10 @@
         <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1067,17 +1067,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1096,10 +1096,10 @@
         <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1107,10 +1107,10 @@
         <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1118,10 +1118,10 @@
         <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1129,10 +1129,10 @@
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1140,10 +1140,10 @@
         <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1151,10 +1151,10 @@
         <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -1162,10 +1162,10 @@
         <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -1173,10 +1173,10 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1184,10 +1184,10 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -1195,10 +1195,10 @@
         <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -1206,10 +1206,10 @@
         <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -1217,10 +1217,10 @@
         <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1228,10 +1228,10 @@
         <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>